<commit_message>
fixing RPS and setting nuclear to not qualify in RPS
</commit_message>
<xml_diff>
--- a/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
+++ b/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\MI\elec\RQSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaggarwal/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/MI/elec/RQSD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F9E344C-A574-40B6-AF0C-E079AF0C7DCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1F5F04-D31D-BA48-AE64-092DF04448A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11535" yWindow="1140" windowWidth="17205" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11540" yWindow="500" windowWidth="17200" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -534,14 +534,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="84.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -552,12 +552,12 @@
         <v>44315</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,55 +565,55 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -631,17 +631,17 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -649,7 +649,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -665,15 +665,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -681,7 +681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -697,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -705,7 +705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -794,13 +794,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -808,7 +808,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -824,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -840,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -856,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -864,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -880,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -888,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -913,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -921,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>

</xml_diff>